<commit_message>
Added mapper and early figs
</commit_message>
<xml_diff>
--- a/data/20190318_excel tsh_2019_data.xlsx
+++ b/data/20190318_excel tsh_2019_data.xlsx
@@ -1,33 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="20910"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simontuke/Dropbox/TSH_2019/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A321F9-8756-024E-BBA4-EA33947A1D51}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="40740" windowHeight="18040"/>
+    <workbookView xWindow="16800" yWindow="460" windowWidth="16800" windowHeight="18960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Nigel Bean</author>
   </authors>
   <commentList>
-    <comment ref="R118" authorId="0">
+    <comment ref="R118" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +57,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I141" authorId="0">
+    <comment ref="I141" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -75,13 +81,13 @@
         </r>
       </text>
     </comment>
-    <comment ref="B225" authorId="0">
+    <comment ref="B225" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
@@ -90,16 +96,25 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-No idea what this means?</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>No idea what this means?</t>
         </r>
       </text>
     </comment>
-    <comment ref="C258" authorId="0">
+    <comment ref="C258" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -123,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C270" authorId="0">
+    <comment ref="C270" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -149,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B310" authorId="0">
+    <comment ref="B310" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -174,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C323" authorId="0">
+    <comment ref="C323" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C352" authorId="0">
+    <comment ref="C352" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -222,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D495" authorId="0">
+    <comment ref="D495" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -248,7 +263,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C499" authorId="0">
+    <comment ref="C499" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D506" authorId="0">
+    <comment ref="D506" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -2459,8 +2474,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2516,6 +2531,19 @@
       <sz val="12"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -3323,7 +3351,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -3375,7 +3403,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -3569,14 +3597,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U510"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -3586,7 +3614,7 @@
       <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" customWidth="1"/>

</xml_diff>